<commit_message>
Added compounding convention into Excel.  Changed the way that strings are converted to some QuantSA types.
</commit_message>
<xml_diff>
--- a/ExcelExamples/FRAExample.xlsx
+++ b/ExcelExamples/FRAExample.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Curves" sheetId="2" r:id="rId2"/>
     <sheet name="TradeInfo&amp;Test" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -146,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -260,10 +261,10 @@
     <xf numFmtId="4" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -570,7 +571,7 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +636,7 @@
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>_xll.QSA.CreateZARFRA(C2,C3,C4,C5,C6,C7)</f>
-        <v>Fra00001.19:37:36-9</v>
+        <v>Fra00001.16:53:54-4</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -653,8 +654,8 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
-        <f ca="1">_xll.QSA.Value(C2&amp;":Value",B10,C13,Curves!B26)</f>
-        <v>Fra00001:Value.19:43:08-16</v>
+        <f>_xll.QSA.Value(C2&amp;":Value",B10,C13,Curves!B26)</f>
+        <v>Fra00001:Value.16:53:54-5</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -662,7 +663,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="12">
-        <f ca="1">_xll.QSA.GetResults(B16,"value")</f>
+        <f>_xll.QSA.GetResults(B16,"value")</f>
         <v>-80.102371743480603</v>
       </c>
     </row>
@@ -712,7 +713,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <f ca="1">ZARFra!C13</f>
+        <f>ZARFra!C13</f>
         <v>42808</v>
       </c>
       <c r="C7" s="9">
@@ -721,7 +722,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <f ca="1">EDATE(B7,10*12)</f>
+        <f>EDATE(B7,10*12)</f>
         <v>46460</v>
       </c>
       <c r="C8" s="9">
@@ -730,8 +731,8 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
-        <f ca="1">_xll.QSA.CreateDatesAndRatesCurve(C3,B7:B8,C7:C8,C4)</f>
-        <v>ZARDiscount.19:43:11-17</v>
+        <f>_xll.QSA.CreateDatesAndRatesCurve(C3,B7:B8,C7:C8,C4)</f>
+        <v>ZARDiscount.16:53:46-1</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="21" x14ac:dyDescent="0.35">
@@ -759,12 +760,12 @@
         <v>16</v>
       </c>
       <c r="D15" s="11" t="str">
-        <f ca="1">B10</f>
-        <v>ZARDiscount.19:43:11-17</v>
+        <f>B10</f>
+        <v>ZARDiscount.16:53:46-1</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f ca="1">_xll.QSA.CreateRateForecastCurveFromDiscount(B15,C15,D15)</f>
-        <v>forecastJIBAR3M.19:43:11-18</v>
+        <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B15,C15,D15)</f>
+        <v>forecastJIBAR3M.16:53:54-2</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -785,8 +786,8 @@
         <v>19</v>
       </c>
       <c r="C20" s="11" t="str">
-        <f ca="1">B10</f>
-        <v>ZARDiscount.19:43:11-17</v>
+        <f>B10</f>
+        <v>ZARDiscount.16:53:46-1</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -794,8 +795,8 @@
         <v>20</v>
       </c>
       <c r="C21" s="11" t="str">
-        <f ca="1">E15</f>
-        <v>forecastJIBAR3M.19:43:11-18</v>
+        <f>E15</f>
+        <v>forecastJIBAR3M.16:53:54-2</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -806,8 +807,8 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
-        <f ca="1">_xll.QSA.CreateCurveModel(C19,C20,C21)</f>
-        <v>curveModel.19:43:11-19</v>
+        <f>_xll.QSA.CreateCurveModel(C19,C20,C21)</f>
+        <v>curveModel.16:53:54-3</v>
       </c>
     </row>
   </sheetData>
@@ -836,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="12">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B2)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B2)</f>
         <v>1000000</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -848,14 +849,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="12">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B3)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B3)</f>
         <v>0.24931506849315069</v>
       </c>
       <c r="F3" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="17">
-        <f ca="1">_xll.QSA.GetDF(Curves!$B$10,C5)</f>
+        <f>_xll.QSA.GetDF(Curves!$B$10,C5)</f>
         <v>0.98091730138860533</v>
       </c>
     </row>
@@ -864,14 +865,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="15">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B4)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B4)</f>
         <v>7.3499999999999996E-2</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
       </c>
       <c r="G4" s="17">
-        <f ca="1">_xll.QSA.GetDF(Curves!$B$10,C6)</f>
+        <f>_xll.QSA.GetDF(Curves!$B$10,C6)</f>
         <v>0.9633461657801673</v>
       </c>
     </row>
@@ -880,14 +881,14 @@
         <v>26</v>
       </c>
       <c r="C5" s="14">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B5)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B5)</f>
         <v>42905</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="16">
-        <f ca="1">EDATE(C5,3)</f>
+        <f>EDATE(C5,3)</f>
         <v>42997</v>
       </c>
     </row>
@@ -896,14 +897,14 @@
         <v>27</v>
       </c>
       <c r="C6" s="14">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B6)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B6)</f>
         <v>42996</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="17">
-        <f ca="1">_xll.QSA.GetDF(Curves!B10,G5)</f>
+        <f>_xll.QSA.GetDF(Curves!B10,G5)</f>
         <v>0.96315483520193168</v>
       </c>
     </row>
@@ -912,14 +913,14 @@
         <v>28</v>
       </c>
       <c r="C7" s="12" t="str">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B7)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B7)</f>
         <v>ZAR:JIBAR:3M</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="17">
-        <f ca="1">(G5-C5)/365</f>
+        <f>(G5-C5)/365</f>
         <v>0.25205479452054796</v>
       </c>
     </row>
@@ -928,14 +929,14 @@
         <v>2</v>
       </c>
       <c r="C8" s="12" t="str">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B8)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B8)</f>
         <v>True</v>
       </c>
       <c r="F8" t="s">
         <v>39</v>
       </c>
       <c r="G8" s="18">
-        <f ca="1">(G3/G6-1)/G7</f>
+        <f>(G3/G6-1)/G7</f>
         <v>7.3166485093756339E-2</v>
       </c>
     </row>
@@ -944,14 +945,14 @@
         <v>29</v>
       </c>
       <c r="C9" s="12" t="str">
-        <f ca="1">_xll.QSA.GetResults(ZARFra!$B$10,B9)</f>
+        <f>_xll.QSA.GetResults(ZARFra!$B$10,B9)</f>
         <v>ZAR</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="17">
-        <f ca="1">(G8-C4)*C2*C3/(1+G8*C3)</f>
+        <f>(G8-C4)*C2*C3/(1+G8*C3)</f>
         <v>-81.660677847241701</v>
       </c>
     </row>
@@ -960,7 +961,7 @@
         <v>35</v>
       </c>
       <c r="G10" s="17">
-        <f ca="1">G9*G3</f>
+        <f>G9*G3</f>
         <v>-80.102371743480589</v>
       </c>
     </row>
@@ -969,7 +970,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="19">
-        <f ca="1">G10-ZARFra!C18</f>
+        <f>G10-ZARFra!C18</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>